<commit_message>
v2.0 base finish the log feature
</commit_message>
<xml_diff>
--- a/20200506 log特征V1.0.xlsx
+++ b/20200506 log特征V1.0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="91">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -116,10 +116,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PS: 不要 区分大小写,都要抓取</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>centos|ubuntu</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,14 +132,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>过滤 Interrupt 。。。。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/var/log/php7.0-fpm.log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>error</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -152,10 +140,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/var/log/apache2/error.log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>apache2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -164,11 +148,220 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>nginx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./nginx/logs/error.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>emerg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>php服务日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apache2日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apache</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apache日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nginx日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mysql</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>warn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VFS  *** too many</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Refuse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Read-only file system</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">dmesg </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">too long </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>too many</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/var/log/php7.0-fpm.log | 其他版本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/var/log/php7.0-fpm.log | 其他版本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>/var/log/httpd/error_log</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>nginx</t>
+    <t xml:space="preserve">/var/log/apache2/error.log </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不数据例外名单，要么攻击，要么密码错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PS: 1. 不要 区分大小写,都要抓取</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PS: 2. err 过滤 Interrupt 。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fail | failure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/var/log/secure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统安全登陆日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">no space left </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统磁盘空间告警</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/var/log/secure
+/var/log/auth.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>core file size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data seg size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scheduling priority</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>file size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pending signals</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max locked memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maxmemory size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">open files </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pipe size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POSIX message queues</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>real-time priority</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stack size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpu time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max user processes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>virtual memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>file locks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/var/log/syslog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/var/log/syslog
+/var/log/messages
+dmesg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ulimit 相关告警</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kernel bash limit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/var/log/mysql/error.log
+systemctl status mysql</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/var/log/mysql/error.log
+systemctl status mysql</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -176,67 +369,24 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>emerg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>php服务日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>apache2日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>apache</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>apache日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nginx日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mysql</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>warn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VFS *** too many</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VFS  *** too many</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Refuse</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>systemctl status mysql</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>systemctl status mysql</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/var/log/mysql/error.log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>drop</t>
+    <t>/var/log/kernel.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/var/log/messages
+dmesg 
+/var/log/syslog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/var/log/messages
+dmesg 
+/var/log/syslog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dmesg 
+ /var/log/dmesg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -274,7 +424,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +440,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -329,14 +485,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -642,42 +810,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.25" style="2" customWidth="1"/>
     <col min="4" max="4" width="25.5" style="2" customWidth="1"/>
-    <col min="5" max="6" width="32.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.75" style="2" customWidth="1"/>
+    <col min="5" max="5" width="32.875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="40.75" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -698,8 +867,8 @@
       <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>25</v>
+      <c r="G2" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -719,8 +888,8 @@
       <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>30</v>
+      <c r="G3" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -778,9 +947,7 @@
       <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -794,10 +961,10 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -813,10 +980,10 @@
         <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -832,10 +999,10 @@
         <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -851,10 +1018,10 @@
         <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -863,7 +1030,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
@@ -882,7 +1049,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
@@ -894,16 +1061,14 @@
       <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
@@ -922,7 +1087,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
@@ -941,7 +1106,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
@@ -960,7 +1125,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
@@ -979,7 +1144,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
@@ -998,7 +1163,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
@@ -1017,7 +1182,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
@@ -1036,7 +1201,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
@@ -1056,16 +1221,16 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1075,16 +1240,16 @@
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1094,16 +1259,16 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1113,16 +1278,16 @@
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -1132,16 +1297,16 @@
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -1151,117 +1316,125 @@
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
+      <c r="B30" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1" t="s">
+      <c r="B31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E31" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1" t="s">
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="E32" s="1" t="s">
-        <v>54</v>
+        <v>19</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="G32" s="1"/>
     </row>
@@ -1270,14 +1443,14 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>15</v>
@@ -1289,14 +1462,14 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>15</v>
@@ -1308,285 +1481,493 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>19</v>
+        <v>49</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="D37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
+      <c r="D39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="1"/>
+      <c r="B44" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D46" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D47" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
-      <c r="B48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D48" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
-      <c r="B49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D49" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="B50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D50" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D51" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
-      <c r="B52" s="1"/>
+      <c r="B52" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D52" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="B53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
-      <c r="B54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D54" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
-      <c r="B55" s="1"/>
+      <c r="B55" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D55" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
-      <c r="B56" s="1"/>
+      <c r="B56" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D56" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
-      <c r="B57" s="1"/>
+      <c r="B57" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D57" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
-      <c r="B58" s="1"/>
+      <c r="B58" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
+      <c r="D58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
-        <v>58</v>
-      </c>
+      <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -1595,9 +1976,7 @@
       <c r="G59" s="1"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
-        <v>59</v>
-      </c>
+      <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -1641,96 +2020,6 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>